<commit_message>
freeCrm keyword driven test framework
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenariosmy.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenariosmy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehrajismayilov/git/KeywordDrivenFramework/KeyDrivenFramework/src/main/java/com/qa/hs/keyword/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3883108C-C38B-594C-A9C4-EF380A45E275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E4AA01-F611-A340-A530-F8D6782F6DC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-420" yWindow="540" windowWidth="25600" windowHeight="14520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>action</t>
   </si>
@@ -73,9 +73,6 @@
     <t>enter url</t>
   </si>
   <si>
-    <t>http://app.hubspot.com/login</t>
-  </si>
-  <si>
     <t>verify sign up link</t>
   </si>
   <si>
@@ -109,18 +106,9 @@
     <t>className</t>
   </si>
   <si>
-    <t>private-page__title</t>
-  </si>
-  <si>
     <t>getText</t>
   </si>
   <si>
-    <t>Sales Dashboard</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
     <t>Mehraj</t>
   </si>
   <si>
@@ -139,10 +127,16 @@
     <t>//input[@type='submit']</t>
   </si>
   <si>
-    <t>//td[text()='CRMPRO']</t>
-  </si>
-  <si>
-    <t>CRMPRO</t>
+    <t>User: Mehraj Ismayilov</t>
+  </si>
+  <si>
+    <t>//td[@class='headertext']</t>
+  </si>
+  <si>
+    <t>headertext</t>
+  </si>
+  <si>
+    <t>https://classic.freecrm.com</t>
   </si>
 </sst>
 </file>
@@ -539,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -557,10 +551,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -583,7 +577,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1">
@@ -600,7 +594,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -608,16 +602,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -625,16 +619,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -642,10 +636,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -656,36 +650,36 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -717,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -734,10 +728,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
@@ -777,18 +771,18 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>3</v>
@@ -816,7 +810,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{8CC4167A-AF2D-5B4B-92B0-952311221A3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>